<commit_message>
Pre Exception Handling Done
</commit_message>
<xml_diff>
--- a/funds/Dipsea/Dipsea_Firm_risk_report_20240404.xlsx
+++ b/funds/Dipsea/Dipsea_Firm_risk_report_20240404.xlsx
@@ -4276,13 +4276,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4820,7 +4820,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="position_liquidity" displayName="position_liquidity" ref="B68:F74" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="position_liquidity" displayName="position_liquidity" ref="B67:F73" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" name="Liquidity" dataDxfId="0"/>
     <tableColumn id="2" name="Long" dataDxfId="0"/>
@@ -7803,43 +7803,60 @@
         <v>0</v>
       </c>
     </row>
+    <row r="67" spans="2:14" ht="16" customHeight="1">
+      <c r="B67" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="68" spans="2:14" ht="16" customHeight="1">
-      <c r="B68" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>81</v>
+      <c r="B68" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="5">
+        <v>0.07468897130248688</v>
+      </c>
+      <c r="D68" s="5">
+        <v>-0.09809265727690714</v>
+      </c>
+      <c r="E68" s="5">
+        <v>0.172781628579394</v>
+      </c>
+      <c r="F68" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="2:14" ht="16" customHeight="1">
       <c r="B69" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C69" s="5">
-        <v>0.07468897130248688</v>
+        <v>0</v>
       </c>
       <c r="D69" s="5">
-        <v>-0.09809265727690714</v>
+        <v>0</v>
       </c>
       <c r="E69" s="5">
-        <v>0.172781628579394</v>
+        <v>0</v>
       </c>
       <c r="F69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:14" ht="16" customHeight="1">
       <c r="B70" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C70" s="5">
         <v>0</v>
@@ -7856,7 +7873,7 @@
     </row>
     <row r="71" spans="2:14" ht="16" customHeight="1">
       <c r="B71" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C71" s="5">
         <v>0</v>
@@ -7873,7 +7890,7 @@
     </row>
     <row r="72" spans="2:14" ht="16" customHeight="1">
       <c r="B72" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C72" s="5">
         <v>0</v>
@@ -7890,7 +7907,7 @@
     </row>
     <row r="73" spans="2:14" ht="16" customHeight="1">
       <c r="B73" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C73" s="5">
         <v>0</v>
@@ -7906,36 +7923,19 @@
       </c>
     </row>
     <row r="74" spans="2:14" ht="16" customHeight="1">
-      <c r="B74" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C74" s="5">
-        <v>0</v>
-      </c>
-      <c r="D74" s="5">
-        <v>0</v>
-      </c>
-      <c r="E74" s="5">
-        <v>0</v>
-      </c>
-      <c r="F74" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:14" ht="16" customHeight="1">
-      <c r="B75" s="7" t="s">
+      <c r="B74" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C74" s="7">
         <v>0.07468897130248688</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D74" s="7">
         <v>-0.09809265727690714</v>
       </c>
-      <c r="E75" s="7">
+      <c r="E74" s="7">
         <v>0.172781628579394</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F74" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>